<commit_message>
oh my god its stable. This combination of lift, drag, and moment coefficients happen to be stable. I do no have a measure of realism but this is a very good sign that a realistic set of coefficients will be stable too.
</commit_message>
<xml_diff>
--- a/Aero design/Flight sim/hover stage sim - RK4 method/lookupTableAlpha.xlsx
+++ b/Aero design/Flight sim/hover stage sim - RK4 method/lookupTableAlpha.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joseph\Documents\Crash-Sat\Crash-Sat\Aero design\Flight sim\hover stage sim - RK4 method\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C08DB68C-86B3-4765-8EB7-ADE3B54B03CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B6B9214-8FE8-4009-BB84-3B500DB098FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="624" yWindow="2160" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4116" yWindow="3732" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -348,96 +348,167 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A14"/>
+  <dimension ref="A1:A31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1">
-        <f>RADIANS(-4)</f>
-        <v>-6.9813170079773182E-2</v>
+        <v>-1.5707963267948966</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2">
-        <f>RADIANS(-3)</f>
-        <v>-5.235987755982989E-2</v>
+        <v>-1.2217304763960306</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3">
-        <f>RADIANS(-2)</f>
-        <v>-3.4906585039886591E-2</v>
+        <v>-0.87266462599716477</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f>RADIANS(-1)</f>
-        <v>-1.7453292519943295E-2</v>
+        <v>-0.52359877559829882</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f>RADIANS(0)</f>
-        <v>0</v>
+        <v>-0.3490658503988659</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6">
-        <f>RADIANS(1)</f>
-        <v>1.7453292519943295E-2</v>
+        <v>-0.17453292519943295</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7">
-        <f>RADIANS(2)</f>
-        <v>3.4906585039886591E-2</v>
+        <v>-0.15707963267948966</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8">
-        <f>RADIANS(3)</f>
-        <v>5.235987755982989E-2</v>
+        <v>-0.13962634015954636</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9">
-        <f>RADIANS(4)</f>
-        <v>6.9813170079773182E-2</v>
+        <v>-0.12217304763960307</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10">
-        <f>RADIANS(5)</f>
-        <v>8.7266462599716474E-2</v>
+        <v>-0.10471975511965978</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11">
-        <f>RADIANS(6)</f>
-        <v>0.10471975511965978</v>
+        <v>-8.7266462599716474E-2</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12">
-        <f>RADIANS(7)</f>
-        <v>0.12217304763960307</v>
+        <v>-6.9813170079773182E-2</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13">
-        <f>RADIANS(8)</f>
-        <v>0.13962634015954636</v>
+        <v>-5.235987755982989E-2</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14">
-        <f>RADIANS(9)</f>
+        <v>-3.4906585039886591E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>-1.7453292519943295E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>1.7453292519943295E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>3.4906585039886591E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>5.235987755982989E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>6.9813170079773182E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>8.7266462599716474E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>0.10471975511965978</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>0.12217304763960307</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>0.13962634015954636</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25">
         <v>0.15707963267948966</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>0.17453292519943295</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>0.3490658503988659</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>0.52359877559829882</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>0.87266462599716477</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>1.2217304763960306</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>1.5707963267948966</v>
       </c>
     </row>
   </sheetData>

</xml_diff>